<commit_message>
Incluindo o link de referência no dataframe para fazer verificações
</commit_message>
<xml_diff>
--- a/docs/respostas_danos_ambientais_df_parte0.xlsx
+++ b/docs/respostas_danos_ambientais_df_parte0.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,11 @@
           <t>valor_multa_diaria</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>link_referencia</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -564,12 +569,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Desmatamento</t>
+          <t>Depósito irregular de madeira</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Depósito irregular de 288,03 metros cúbicos de madeira em tora sem licença válida, constatado em 30/04/2016.</t>
+          <t>A empresa mantinha em depósito 288,03 metros cúbicos de madeira em tora sem licença válida.</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -595,8 +600,10 @@
           <t>Custas Judiciais e Acordos</t>
         </is>
       </c>
-      <c r="P2" t="n">
-        <v>0</v>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -606,6 +613,11 @@
       <c r="R2" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/0cacd6d80c499ae25dcb85380a07c3dd.pdf</t>
         </is>
       </c>
     </row>
@@ -648,12 +660,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Desmatamento de APP</t>
+          <t>Desmatamento de vegetação nativa</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Destruição de 121,15 hectares de floresta nativa na Amazônia sem autorização, embargando a área para evitar uso com bovinos e buscando regeneração natural.</t>
+          <t>Destruição de 121,15 hectares de floresta nativa no bioma amazônico sem autorização da autoridade ambiental.</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -690,6 +702,11 @@
       <c r="R3" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/90df1f9ac9917f6df4b9f91915b3a8bd.pdf</t>
         </is>
       </c>
     </row>
@@ -732,7 +749,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Lançamento e queima de rejeitos de indústria madeireira</t>
+          <t>Queima de Rejeitos Industriais</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -768,12 +785,17 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>24240.00</t>
+          <t>NULL</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
           <t>10000.00</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/209b98634c9c4a3f7c83d1c521c5b8d6.pdf</t>
         </is>
       </c>
     </row>
@@ -821,7 +843,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Ação Civil Pública movida por desmatamento e impedimento da regeneração da cobertura florestal explorada.</t>
+          <t>Ação civil pública movida por desmatamento e impedimento da regeneração da cobertura florestal explorada.</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -847,10 +869,8 @@
           <t>NULL</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="P5" t="n">
+        <v>0</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -860,6 +880,11 @@
       <c r="R5" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/7cef4bd654c356d84d7a617351f802cc.pdf</t>
         </is>
       </c>
     </row>
@@ -907,7 +932,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Supressão de castanhais, poluição hídrica do Rio Itacaiúnas e Igarapé Salobo devido à atividade minerária do Projeto Salobo, impactando comunidades indígenas Xikrin.</t>
+          <t>Supressão de castanheiras, poluição hídrica do Rio Itacaiúnas e Igarapé Salobo, impactos na Floresta Nacional do Tapirapé-Aquiri e nas comunidades indígenas Xikrin.</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -917,25 +942,25 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>54000</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>m2</t>
         </is>
       </c>
       <c r="N6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Obrigações de Fazer (com custo)</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -946,6 +971,11 @@
       <c r="R6" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/d5d876cd4f1b1b52385f1ec4df9886ba.html</t>
         </is>
       </c>
     </row>
@@ -1032,6 +1062,11 @@
           <t>100000.00</t>
         </is>
       </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/24586eb78e174455c03d488d6518e16c.html</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1103,10 +1138,8 @@
           <t>Custas Judiciais e Acordos</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="P8" t="n">
+        <v>0</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
@@ -1116,6 +1149,11 @@
       <c r="R8" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/be70db0dae0a1d1f18eb65dfd5523e76.html</t>
         </is>
       </c>
     </row>
@@ -1158,12 +1196,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Interrupção no fornecimento de energia elétrica</t>
+          <t>Falha no fornecimento de energia elétrica</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Interrupções sucessivas e prolongadas no fornecimento de energia elétrica, causando danos materiais e morais ao usuário.</t>
+          <t>Falhas no fornecimento de energia elétrica que causaram gastos com geradores e substituição de equipamentos.</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1182,7 +1220,7 @@
         </is>
       </c>
       <c r="N9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1200,6 +1238,11 @@
       <c r="R9" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/5631abc57e085f5121b0ead2d78e9e85.html</t>
         </is>
       </c>
     </row>
@@ -1242,12 +1285,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Ocupação Irregular de Terreno</t>
+          <t>Ocupação Irregular de Terreno de Marinha</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Ocupação irregular de barraca de praia em terreno de marinha, sem licença, impactando o acesso público e o meio ambiente local.</t>
+          <t>Ocupação irregular de barraca de praia em terreno de marinha, sem licença, impactando o acesso público e o meio ambiente.</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1262,7 +1305,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>m2</t>
         </is>
       </c>
       <c r="N10" t="b">
@@ -1274,7 +1317,7 @@
         </is>
       </c>
       <c r="P10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
@@ -1284,6 +1327,11 @@
       <c r="R10" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/a322a1e63179ad2a721b9268801dbfb6.pdf</t>
         </is>
       </c>
     </row>
@@ -1331,7 +1379,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Emissão de ruídos acima dos limites permitidos pela NBR 10.151, causando perturbação aos moradores vizinhos.</t>
+          <t>Emissão de som em violação aos limites de horário e decibéis permitidos pela legislação, causando transtornos aos moradores do entorno.</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1350,15 +1398,17 @@
         </is>
       </c>
       <c r="N11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Multas Administrativas</t>
-        </is>
-      </c>
-      <c r="P11" t="n">
-        <v>2</v>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
@@ -1367,7 +1417,12 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>1000.00</t>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/f8941539197bdd583e3bdd448abb2e6c.html</t>
         </is>
       </c>
     </row>
@@ -1410,17 +1465,17 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Publicidade Enganosa e Atraso na Entrega de Imóvel</t>
+          <t>Descumprimento de contrato</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Atraso de 339 dias na entrega de imóvel e divergências entre o prometido na venda e o entregue, incluindo mobiliário e áreas de convivência em desacordo.</t>
+          <t>Atraso na entrega de imóvel e divergências entre o que foi vendido e o que foi efetivamente entregue, causando prejuízos aos compradores.</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>29/12/2013</t>
+          <t>NULL</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1434,7 +1489,7 @@
         </is>
       </c>
       <c r="N12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1452,6 +1507,11 @@
       <c r="R12" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/c7fac8749343a02deddd5dfdcb5092e1.html</t>
         </is>
       </c>
     </row>
@@ -1494,17 +1554,17 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Infraestrutura Irregular</t>
+          <t>Danos ao sistema de saneamento</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Atraso na entrega de obras de infraestrutura, especificamente a rede de distribuição de água potável, causando transtornos ao comprador do lote.</t>
+          <t>Atraso na entrega de infraestrutura básica, como rede de água potável, resultando em uso de poço artesiano pelo comprador e falta de rede de esgoto sanitário.</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>22/03/2016</t>
+          <t>07/03/2017</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1518,11 +1578,11 @@
         </is>
       </c>
       <c r="N13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Obrigações de Fazer (com custo)</t>
+          <t>NULL</t>
         </is>
       </c>
       <c r="P13" t="n">
@@ -1536,6 +1596,11 @@
       <c r="R13" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/179ce549bff6f6044d73c9c6f7b54d98.html</t>
         </is>
       </c>
     </row>
@@ -1578,12 +1643,12 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Abastecimento Irregular de Água</t>
+          <t>Abastecimento irregular de água</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Abastecimento irregular de água afetando moradores do Bairro Jorge Texeira, com fornecimento máximo de três horas diárias, chegando a trinta minutos.</t>
+          <t>Abastecimento irregular de água no bairro Jorge Texeira, com fornecimento de água de no máximo três horas diárias, passando a trinta minutos.</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1606,7 +1671,7 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>NULL</t>
+          <t>Custas Judiciais e Acordos</t>
         </is>
       </c>
       <c r="P14" t="n">
@@ -1620,6 +1685,11 @@
       <c r="R14" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/e50aea65864c6a6ca7ab8ab06025d54f.pdf</t>
         </is>
       </c>
     </row>
@@ -1662,12 +1732,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Abastecimento irregular de água</t>
+          <t>Abastecimento Irregular de Água</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Abastecimento irregular de água no Bairro Jorge Texeira, com fornecimento descontínuo e precário, afetando moradores da região.</t>
+          <t>Abastecimento de água irregular no bairro Jorge Teixeira, com fornecimento descontínuo e precário, afetando moradores e causando transtornos.</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1704,6 +1774,11 @@
       <c r="R15" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/c9c4529e46b75ee5e400e42350f2b2d7.pdf</t>
         </is>
       </c>
     </row>
@@ -1746,17 +1821,17 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Interrupção no fornecimento de água</t>
+          <t>Poluição Hídrica</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Interrupção do fornecimento de água por 3 dias devido ao rompimento de um encanamento pertencente à empresa ré.</t>
+          <t>Interrupção no fornecimento de água por 3 dias devido ao rompimento de um encanamento.</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>20/02/24</t>
+          <t>20/02/2024</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1770,7 +1845,7 @@
         </is>
       </c>
       <c r="N16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1788,6 +1863,11 @@
       <c r="R16" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/4a966dbc383fe11597026e3ca7432c93.pdf</t>
         </is>
       </c>
     </row>
@@ -1835,7 +1915,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Desmate de 11,826 hectares de Floresta Estacional Semidecidual com tipologia de regeneração do Bioma Mata Atlântica, sem a devida autorização ambiental.</t>
+          <t>Desmate de 11,826 hectares de Floresta Estacional Semidecidual, Bioma Mata Atlântica, sem autorização ambiental na Fazenda Manancial, zona rural de Águas Vermelhas.</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1862,7 +1942,7 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
@@ -1871,7 +1951,12 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>500.00</t>
+          <t>NULL</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/e448073edc85a7c3dd335c89e2c64c2e.html</t>
         </is>
       </c>
     </row>
@@ -1914,12 +1999,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Desmatamento de APP</t>
+          <t>Desmatamento de vegetação nativa</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Supressão de 30 árvores nativas, depositadas em área de preservação permanente, impedindo a regeneração natural.</t>
+          <t>Supressão de 30 árvores nativas sem licença, depositadas em APP, impedindo regeneração. Regeneração natural ocorrida, mas compensação necessária.</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1956,6 +2041,11 @@
       <c r="R18" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/4af9d082c1a6dd5841a9c871eb76b26b.html</t>
         </is>
       </c>
     </row>
@@ -2003,7 +2093,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Captação irregular de água do Rio Verde para obras de loteamento, impactando a disponibilidade hídrica e APP.</t>
+          <t>Captação irregular de água do Rio Verde para obras de loteamento, causando dano ambiental pontual e de pequena monta.</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2040,6 +2130,11 @@
       <c r="R19" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/cbdda0e55f226a6f1eac06b4a819d143.html</t>
         </is>
       </c>
     </row>
@@ -2082,12 +2177,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Danos a poste de energia elétrica</t>
+          <t>Colisão de veículo contra poste de energia elétrica</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Colisão de veículo com poste de energia elétrica devido à negligência do condutor, causando danos materiais ao veículo e ao poste.</t>
+          <t>O veículo colidiu contra um poste de energia elétrica na Praça Universitária, danificando o veículo locado.</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -2124,6 +2219,11 @@
       <c r="R20" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/e748a98ec567a8446cf05d6974c9d6d5.html</t>
         </is>
       </c>
     </row>
@@ -2171,7 +2271,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Aterramento de nascente e intervenção em área de preservação permanente (APP) devido à instalação de atividade sem autorização.</t>
+          <t>Aterramento de nascente e intervenção em área de preservação permanente (APP) de aproximadamente 4 hectares e intervenção em curso d’água sem outorga.</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2208,6 +2308,11 @@
       <c r="R21" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/02597b35d5e8ece30d36627f30550386.html</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2360,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Assoreamento do leito do Córrego Canta Galo devido a deslizamento de talude, causando erosão e prejuízo ao meio ambiente.</t>
+          <t>Assoreamento do leito do Córrego Canta Galo devido a deslizamento de talude e erosão.</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2281,8 +2386,10 @@
           <t>Obrigações de Fazer (com custo)</t>
         </is>
       </c>
-      <c r="P22" t="n">
-        <v>0</v>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
@@ -2292,6 +2399,11 @@
       <c r="R22" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/7d54d2fd28f74c625bb2157b3d507fe6.html</t>
         </is>
       </c>
     </row>
@@ -2376,6 +2488,11 @@
       <c r="R23" t="inlineStr">
         <is>
           <t>NULL</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>http://jud-anexos.digesto.com.br/fab3efa39a57f1d1a8bd1457980931ab.html</t>
         </is>
       </c>
     </row>

</xml_diff>